<commit_message>
upload Wyoming water rights data
</commit_message>
<xml_diff>
--- a/Design_docs/SampleInputData/WaDE2_CVs.xlsx
+++ b/Design_docs/SampleInputData/WaDE2_CVs.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317D2FAC-CF1A-472E-AF5A-A3ADDAB8FB94}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87794CB2-2E04-485B-A5F3-E6F7B91D69AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="729" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="729" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAICSCode" sheetId="1" r:id="rId1"/>
     <sheet name="Variable" sheetId="11" r:id="rId2"/>
     <sheet name="VariableSpecific" sheetId="15" r:id="rId3"/>
     <sheet name="ReportYearCV" sheetId="2" r:id="rId4"/>
-    <sheet name="LegalStatusCode" sheetId="3" r:id="rId5"/>
+    <sheet name="LegalStatus" sheetId="3" r:id="rId5"/>
     <sheet name="GNISCode" sheetId="4" r:id="rId6"/>
     <sheet name="NHDNetworkStatus" sheetId="5" r:id="rId7"/>
     <sheet name="NHDProduct" sheetId="20" r:id="rId8"/>
@@ -28,6 +28,7 @@
     <sheet name="RegulatoryStatus" sheetId="19" r:id="rId18"/>
     <sheet name="CropType" sheetId="17" r:id="rId19"/>
     <sheet name="IrrigationMethod" sheetId="18" r:id="rId20"/>
+    <sheet name="WaterRightType" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="188">
   <si>
     <t>Term</t>
   </si>
@@ -154,18 +155,6 @@
     <t>AllocationAll</t>
   </si>
   <si>
-    <t>Absolute</t>
-  </si>
-  <si>
-    <t>Conditional</t>
-  </si>
-  <si>
-    <t>Conditional Absolute</t>
-  </si>
-  <si>
-    <t>ConditionalAbsolute</t>
-  </si>
-  <si>
     <t>https://geonames.usgs.gov/domestic/index.html</t>
   </si>
   <si>
@@ -458,13 +447,202 @@
   </si>
   <si>
     <t>NHD Product that is used for the indexing. Shouldbe NHDPlus V1, NHDPlus V2, NHD Med Res, or NHD High Res.</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Adjudication Decree</t>
+  </si>
+  <si>
+    <t>Adverse Use</t>
+  </si>
+  <si>
+    <t>Application to Appropriate</t>
+  </si>
+  <si>
+    <t>Decree</t>
+  </si>
+  <si>
+    <t>Diligence Claim</t>
+  </si>
+  <si>
+    <t>Federal Reserved Water Right</t>
+  </si>
+  <si>
+    <t>Fixed-Time Application</t>
+  </si>
+  <si>
+    <t>Pending Adjudication Claim</t>
+  </si>
+  <si>
+    <t>Water Company Shares</t>
+  </si>
+  <si>
+    <t>Temporary Application</t>
+  </si>
+  <si>
+    <t>Underground Water Claim</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>ADEC_UT</t>
+  </si>
+  <si>
+    <t>ADV_UT</t>
+  </si>
+  <si>
+    <t>APPL_UT</t>
+  </si>
+  <si>
+    <t>DEC_UT</t>
+  </si>
+  <si>
+    <t>DIL_UT</t>
+  </si>
+  <si>
+    <t>FEDR_UT</t>
+  </si>
+  <si>
+    <t>FIXD_UT</t>
+  </si>
+  <si>
+    <t>PAC_UT</t>
+  </si>
+  <si>
+    <t>SHAR_UT</t>
+  </si>
+  <si>
+    <t>TEMP_UT</t>
+  </si>
+  <si>
+    <t>UGWC_UT</t>
+  </si>
+  <si>
+    <t>NoStatus_UT</t>
+  </si>
+  <si>
+    <t>do NOT have a Status</t>
+  </si>
+  <si>
+    <t>No status</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>Certificated</t>
+  </si>
+  <si>
+    <t>Disallowed</t>
+  </si>
+  <si>
+    <t>Expired</t>
+  </si>
+  <si>
+    <t>Forfeited</t>
+  </si>
+  <si>
+    <t>Lapsed</t>
+  </si>
+  <si>
+    <t>Lapsed(Destroyed), Currently NOT Used</t>
+  </si>
+  <si>
+    <t>No Proof Required</t>
+  </si>
+  <si>
+    <t>Nonuse</t>
+  </si>
+  <si>
+    <t>Perfected</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Rejected(Destroyed), Currently Not Used</t>
+  </si>
+  <si>
+    <t>Renumbered</t>
+  </si>
+  <si>
+    <t>Terminated</t>
+  </si>
+  <si>
+    <t>Unapproved</t>
+  </si>
+  <si>
+    <t>Withdrawn</t>
+  </si>
+  <si>
+    <t>Withdrawn(Destroyed), Currently Not Used</t>
+  </si>
+  <si>
+    <t>Water User`s Claim</t>
+  </si>
+  <si>
+    <t>APP_UT</t>
+  </si>
+  <si>
+    <t>CERT_UT</t>
+  </si>
+  <si>
+    <t>DIS_UT</t>
+  </si>
+  <si>
+    <t>EXP_UT</t>
+  </si>
+  <si>
+    <t>FORF_UT</t>
+  </si>
+  <si>
+    <t>LAP_UT</t>
+  </si>
+  <si>
+    <t>LAPD_UT</t>
+  </si>
+  <si>
+    <t>NPR_UT</t>
+  </si>
+  <si>
+    <t>NUSE_UT</t>
+  </si>
+  <si>
+    <t>PERF_UT</t>
+  </si>
+  <si>
+    <t>REJ_UT</t>
+  </si>
+  <si>
+    <t>REJD_UT</t>
+  </si>
+  <si>
+    <t>RNUM_UT</t>
+  </si>
+  <si>
+    <t>TERM_UT</t>
+  </si>
+  <si>
+    <t>UNAP_UT</t>
+  </si>
+  <si>
+    <t>WD_UT</t>
+  </si>
+  <si>
+    <t>WDD_UT</t>
+  </si>
+  <si>
+    <t>WUC_UT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -557,6 +735,12 @@
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -630,7 +814,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
@@ -685,6 +869,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -969,7 +1157,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1323,7 @@
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1146,7 +1334,7 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1220,35 +1408,35 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1322,46 +1510,46 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1441,12 +1629,12 @@
         <v>4326</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G3" s="12"/>
     </row>
@@ -1521,26 +1709,26 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1614,13 +1802,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1694,308 +1882,308 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
@@ -2072,18 +2260,18 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2096,7 +2284,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2157,13 +2345,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2237,13 +2425,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2410,13 +2598,244 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>124</v>
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7A25EA-9584-42A7-8F0F-E1923979A8E4}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2803,54 +3222,58 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA2232C-C31D-4873-896B-D37A11CE5BF2}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
+      <c r="C2" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -2861,36 +3284,292 @@
       <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>27</v>
+        <v>149</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>28</v>
+        <v>138</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+        <v>152</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>169</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2970,10 +3649,10 @@
         <v>1442221</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -3047,13 +3726,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -3128,13 +3807,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3144,54 +3823,58 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2779408E-E89A-485C-9D84-C0725F0A26DB}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
+      <c r="C2" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -3202,19 +3885,25 @@
       <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>33</v>
+      <c r="C3" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>